<commit_message>
milp + reformulate raw material buying
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -15,6 +15,9 @@
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
     <sheet name="Inventory" r:id="rId5" sheetId="2"/>
+    <sheet name="RawMaterial" r:id="rId6" sheetId="3"/>
+    <sheet name="RawMaterialInventory" r:id="rId7" sheetId="4"/>
+    <sheet name="PMRunning" r:id="rId8" sheetId="5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Product</t>
   </si>
@@ -65,6 +68,15 @@
   </si>
   <si>
     <t>M2</t>
+  </si>
+  <si>
+    <t>RawMaterial</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Running</t>
   </si>
 </sst>
 </file>
@@ -453,7 +465,7 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>478.0</v>
+        <v>510.0000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -470,7 +482,7 @@
         <v>7</v>
       </c>
       <c r="E3">
-        <v>222.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -759,7 +771,7 @@
         <v>7</v>
       </c>
       <c r="E20">
-        <v>0.0</v>
+        <v>170.00000000000068</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -793,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="E22">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -827,7 +839,7 @@
         <v>7</v>
       </c>
       <c r="E24">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -861,7 +873,7 @@
         <v>9</v>
       </c>
       <c r="E26">
-        <v>522.0</v>
+        <v>489.9999999999994</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1133,7 +1145,7 @@
         <v>9</v>
       </c>
       <c r="E42">
-        <v>0.0</v>
+        <v>1.0231815394945443e-12</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1167,7 +1179,7 @@
         <v>9</v>
       </c>
       <c r="E44">
-        <v>0.0</v>
+        <v>251.9999999999991</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1201,7 +1213,7 @@
         <v>9</v>
       </c>
       <c r="E46">
-        <v>0.0</v>
+        <v>989.9999999999998</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1235,7 +1247,7 @@
         <v>9</v>
       </c>
       <c r="E48">
-        <v>0.0</v>
+        <v>990.0000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1333,7 +1345,7 @@
         <v>7</v>
       </c>
       <c r="E4">
-        <v>0.0</v>
+        <v>500.00000000000034</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1350,7 +1362,7 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <v>690.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1367,7 +1379,7 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>590.0</v>
+        <v>399.99999999999994</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1401,7 +1413,7 @@
         <v>7</v>
       </c>
       <c r="E8">
-        <v>490.0</v>
+        <v>300.0000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1435,7 +1447,7 @@
         <v>7</v>
       </c>
       <c r="E10">
-        <v>470.0</v>
+        <v>280.00000000000034</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1469,7 +1481,7 @@
         <v>7</v>
       </c>
       <c r="E12">
-        <v>0.0</v>
+        <v>270.00000000000034</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1486,7 +1498,7 @@
         <v>7</v>
       </c>
       <c r="E13">
-        <v>460.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1503,7 +1515,7 @@
         <v>7</v>
       </c>
       <c r="E14">
-        <v>450.0</v>
+        <v>260.00000000000034</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1537,7 +1549,7 @@
         <v>7</v>
       </c>
       <c r="E16">
-        <v>0.0</v>
+        <v>250.00000000000034</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1554,7 +1566,7 @@
         <v>7</v>
       </c>
       <c r="E17">
-        <v>440.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1571,7 +1583,7 @@
         <v>7</v>
       </c>
       <c r="E18">
-        <v>0.0</v>
+        <v>150.00000000000034</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1588,7 +1600,7 @@
         <v>7</v>
       </c>
       <c r="E19">
-        <v>340.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1605,7 +1617,7 @@
         <v>7</v>
       </c>
       <c r="E20">
-        <v>190.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1656,7 +1668,7 @@
         <v>7</v>
       </c>
       <c r="E23">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1673,7 +1685,7 @@
         <v>7</v>
       </c>
       <c r="E24">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1775,7 +1787,7 @@
         <v>9</v>
       </c>
       <c r="E30">
-        <v>512.0</v>
+        <v>479.9999999999994</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1809,7 +1821,7 @@
         <v>9</v>
       </c>
       <c r="E32">
-        <v>0.0</v>
+        <v>469.9999999999994</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1826,7 +1838,7 @@
         <v>9</v>
       </c>
       <c r="E33">
-        <v>502.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1843,7 +1855,7 @@
         <v>9</v>
       </c>
       <c r="E34">
-        <v>402.0</v>
+        <v>369.99999999999966</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1877,7 +1889,7 @@
         <v>9</v>
       </c>
       <c r="E36">
-        <v>0.0</v>
+        <v>269.99999999999943</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1894,7 +1906,7 @@
         <v>9</v>
       </c>
       <c r="E37">
-        <v>302.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1911,7 +1923,7 @@
         <v>9</v>
       </c>
       <c r="E38">
-        <v>0.0</v>
+        <v>169.99999999999943</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1928,7 +1940,7 @@
         <v>9</v>
       </c>
       <c r="E39">
-        <v>202.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1945,7 +1957,7 @@
         <v>9</v>
       </c>
       <c r="E40">
-        <v>0.0</v>
+        <v>69.99999999999945</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1962,7 +1974,7 @@
         <v>9</v>
       </c>
       <c r="E41">
-        <v>102.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1979,7 +1991,7 @@
         <v>9</v>
       </c>
       <c r="E42">
-        <v>92.0</v>
+        <v>59.99999999999909</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2013,7 +2025,7 @@
         <v>9</v>
       </c>
       <c r="E44">
-        <v>82.0</v>
+        <v>49.999999999999446</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2064,7 +2076,7 @@
         <v>9</v>
       </c>
       <c r="E47">
-        <v>32.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2081,7 +2093,7 @@
         <v>9</v>
       </c>
       <c r="E48">
-        <v>22.0</v>
+        <v>241.9999999999991</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2115,7 +2127,7 @@
         <v>9</v>
       </c>
       <c r="E50">
-        <v>10.0</v>
+        <v>999.9999999999998</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2132,7 +2144,7 @@
         <v>9</v>
       </c>
       <c r="E51">
-        <v>0.0</v>
+        <v>219.99999999999915</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2149,7 +2161,7 @@
         <v>9</v>
       </c>
       <c r="E52">
-        <v>0.0</v>
+        <v>1000.0000000000005</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2166,6 +2178,590 @@
         <v>9</v>
       </c>
       <c r="E53">
+        <v>1199.9999999999986</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>202201</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>499.9999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>202202</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>202203</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>-2.335909243811332e-13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>202204</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>202205</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>202206</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>202207</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>202208</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>2.8421709430404007e-13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>202209</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>6.821210263296962e-13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>202210</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>210.9999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>202211</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>499.9999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>202212</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>500.0000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>202200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>202201</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>202202</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>5.684341886080801e-13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>202203</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>202204</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>202205</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>202206</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>202207</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>202208</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>202209</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>202210</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>202211</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>202212</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>202200</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>202201</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>202202</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>202203</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>202204</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>202205</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>202206</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>202207</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>202208</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>202209</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>202210</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>202211</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>202212</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
at least its running
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Thesis\dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753993D9-4F02-437F-B240-5219934C4AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
-    <sheet name="Inventory" sheetId="2" r:id="rId2"/>
-    <sheet name="RawMaterial" sheetId="3" r:id="rId3"/>
-    <sheet name="RawMaterialInventory" sheetId="4" r:id="rId4"/>
-    <sheet name="PMRunning" sheetId="5" r:id="rId5"/>
-    <sheet name="Contracts" sheetId="6" r:id="rId6"/>
-    <sheet name="RawMaterialContract" sheetId="7" r:id="rId7"/>
+    <sheet name="Inventory" r:id="rId5" sheetId="2"/>
+    <sheet name="RawMaterial" r:id="rId6" sheetId="3"/>
+    <sheet name="RawMaterialInventory" r:id="rId7" sheetId="4"/>
+    <sheet name="PMRunning" r:id="rId8" sheetId="5"/>
+    <sheet name="Contracts" r:id="rId9" sheetId="6"/>
+    <sheet name="RawMaterialContract" r:id="rId10" sheetId="7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Product</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>BULK</t>
+  </si>
+  <si>
+    <t>FD</t>
   </si>
 </sst>
 </file>
@@ -444,16 +447,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B778F3-2102-470C-8644-C8B3EED064B7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -484,10 +485,10 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -501,10 +502,10 @@
         <v>7</v>
       </c>
       <c r="E3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9.999999999999773</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -518,10 +519,10 @@
         <v>7</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -535,10 +536,10 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -552,10 +553,10 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -569,10 +570,10 @@
         <v>7</v>
       </c>
       <c r="E7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -586,10 +587,10 @@
         <v>7</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -603,10 +604,10 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -620,10 +621,10 @@
         <v>7</v>
       </c>
       <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -637,10 +638,10 @@
         <v>7</v>
       </c>
       <c r="E11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -654,10 +655,10 @@
         <v>7</v>
       </c>
       <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -671,10 +672,10 @@
         <v>7</v>
       </c>
       <c r="E13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -688,10 +689,10 @@
         <v>7</v>
       </c>
       <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -705,10 +706,10 @@
         <v>7</v>
       </c>
       <c r="E15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -722,10 +723,10 @@
         <v>7</v>
       </c>
       <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -739,10 +740,10 @@
         <v>7</v>
       </c>
       <c r="E17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -756,10 +757,10 @@
         <v>7</v>
       </c>
       <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -773,10 +774,10 @@
         <v>7</v>
       </c>
       <c r="E19">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -790,10 +791,10 @@
         <v>7</v>
       </c>
       <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -807,10 +808,10 @@
         <v>7</v>
       </c>
       <c r="E21">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>170.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -824,10 +825,10 @@
         <v>7</v>
       </c>
       <c r="E22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -841,10 +842,10 @@
         <v>7</v>
       </c>
       <c r="E23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -858,10 +859,10 @@
         <v>7</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -875,10 +876,10 @@
         <v>7</v>
       </c>
       <c r="E25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -892,10 +893,10 @@
         <v>9</v>
       </c>
       <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -909,10 +910,10 @@
         <v>9</v>
       </c>
       <c r="E27">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -926,10 +927,10 @@
         <v>9</v>
       </c>
       <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -943,10 +944,10 @@
         <v>9</v>
       </c>
       <c r="E29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -960,10 +961,10 @@
         <v>9</v>
       </c>
       <c r="E30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -977,10 +978,10 @@
         <v>9</v>
       </c>
       <c r="E31">
-        <v>99.999999999999986</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -994,10 +995,10 @@
         <v>9</v>
       </c>
       <c r="E32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1011,10 +1012,10 @@
         <v>9</v>
       </c>
       <c r="E33">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1028,10 +1029,10 @@
         <v>9</v>
       </c>
       <c r="E34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1045,10 +1046,10 @@
         <v>9</v>
       </c>
       <c r="E35">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1062,10 +1063,10 @@
         <v>9</v>
       </c>
       <c r="E36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1079,10 +1080,10 @@
         <v>9</v>
       </c>
       <c r="E37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1096,10 +1097,10 @@
         <v>9</v>
       </c>
       <c r="E38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1113,10 +1114,10 @@
         <v>9</v>
       </c>
       <c r="E39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1130,10 +1131,10 @@
         <v>9</v>
       </c>
       <c r="E40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1147,10 +1148,10 @@
         <v>9</v>
       </c>
       <c r="E41">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -1164,10 +1165,10 @@
         <v>9</v>
       </c>
       <c r="E42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1181,10 +1182,10 @@
         <v>9</v>
       </c>
       <c r="E43">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1198,10 +1199,10 @@
         <v>9</v>
       </c>
       <c r="E44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1215,10 +1216,10 @@
         <v>9</v>
       </c>
       <c r="E45">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -1232,10 +1233,10 @@
         <v>9</v>
       </c>
       <c r="E46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1249,10 +1250,10 @@
         <v>9</v>
       </c>
       <c r="E47">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1266,10 +1267,10 @@
         <v>9</v>
       </c>
       <c r="E48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1283,7 +1284,7 @@
         <v>9</v>
       </c>
       <c r="E49">
-        <v>10</v>
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>
@@ -1292,14 +1293,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC628001-816A-440F-AEEF-A5E0DC3E6ADE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1316,7 +1317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1330,10 +1331,10 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1347,10 +1348,10 @@
         <v>7</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1364,10 +1365,10 @@
         <v>7</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1381,10 +1382,10 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1398,10 +1399,10 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1415,10 +1416,10 @@
         <v>7</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1432,10 +1433,10 @@
         <v>7</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1449,10 +1450,10 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1466,10 +1467,10 @@
         <v>7</v>
       </c>
       <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1483,10 +1484,10 @@
         <v>7</v>
       </c>
       <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1500,10 +1501,10 @@
         <v>7</v>
       </c>
       <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1517,10 +1518,10 @@
         <v>7</v>
       </c>
       <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1534,10 +1535,10 @@
         <v>7</v>
       </c>
       <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1551,10 +1552,10 @@
         <v>7</v>
       </c>
       <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1568,10 +1569,10 @@
         <v>7</v>
       </c>
       <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1585,10 +1586,10 @@
         <v>7</v>
       </c>
       <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1602,10 +1603,10 @@
         <v>7</v>
       </c>
       <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1619,10 +1620,10 @@
         <v>7</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1636,10 +1637,10 @@
         <v>7</v>
       </c>
       <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1653,10 +1654,10 @@
         <v>7</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1670,10 +1671,10 @@
         <v>7</v>
       </c>
       <c r="E22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1687,10 +1688,10 @@
         <v>7</v>
       </c>
       <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1704,10 +1705,10 @@
         <v>7</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1721,10 +1722,10 @@
         <v>7</v>
       </c>
       <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1738,10 +1739,10 @@
         <v>7</v>
       </c>
       <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1755,10 +1756,10 @@
         <v>7</v>
       </c>
       <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1772,10 +1773,10 @@
         <v>9</v>
       </c>
       <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1789,10 +1790,10 @@
         <v>9</v>
       </c>
       <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1806,10 +1807,10 @@
         <v>9</v>
       </c>
       <c r="E30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1823,10 +1824,10 @@
         <v>9</v>
       </c>
       <c r="E31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1840,10 +1841,10 @@
         <v>9</v>
       </c>
       <c r="E32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1857,10 +1858,10 @@
         <v>9</v>
       </c>
       <c r="E33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1874,10 +1875,10 @@
         <v>9</v>
       </c>
       <c r="E34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1891,10 +1892,10 @@
         <v>9</v>
       </c>
       <c r="E35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1908,10 +1909,10 @@
         <v>9</v>
       </c>
       <c r="E36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1925,10 +1926,10 @@
         <v>9</v>
       </c>
       <c r="E37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1942,10 +1943,10 @@
         <v>9</v>
       </c>
       <c r="E38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1959,10 +1960,10 @@
         <v>9</v>
       </c>
       <c r="E39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1976,10 +1977,10 @@
         <v>9</v>
       </c>
       <c r="E40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1993,10 +1994,10 @@
         <v>9</v>
       </c>
       <c r="E41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -2010,10 +2011,10 @@
         <v>9</v>
       </c>
       <c r="E42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -2027,10 +2028,10 @@
         <v>9</v>
       </c>
       <c r="E43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -2044,10 +2045,10 @@
         <v>9</v>
       </c>
       <c r="E44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -2061,10 +2062,10 @@
         <v>9</v>
       </c>
       <c r="E45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -2078,10 +2079,10 @@
         <v>9</v>
       </c>
       <c r="E46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -2095,10 +2096,10 @@
         <v>9</v>
       </c>
       <c r="E47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -2112,10 +2113,10 @@
         <v>9</v>
       </c>
       <c r="E48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -2129,10 +2130,10 @@
         <v>9</v>
       </c>
       <c r="E49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -2146,10 +2147,10 @@
         <v>9</v>
       </c>
       <c r="E50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -2163,10 +2164,10 @@
         <v>9</v>
       </c>
       <c r="E51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -2180,10 +2181,10 @@
         <v>9</v>
       </c>
       <c r="E52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>9</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -2206,14 +2207,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736FC485-59F2-44BD-9AE0-3234E4188366}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2224,7 +2225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>202201</v>
       </c>
@@ -2232,10 +2233,10 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>202202</v>
       </c>
@@ -2243,10 +2244,10 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45.999999999999886</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>202203</v>
       </c>
@@ -2254,10 +2255,10 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>202204</v>
       </c>
@@ -2265,10 +2266,10 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>202205</v>
       </c>
@@ -2276,10 +2277,10 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>202206</v>
       </c>
@@ -2287,10 +2288,10 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>202207</v>
       </c>
@@ -2298,10 +2299,10 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>202208</v>
       </c>
@@ -2309,10 +2310,10 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>202209</v>
       </c>
@@ -2320,10 +2321,10 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>202210</v>
       </c>
@@ -2331,10 +2332,10 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>202211</v>
       </c>
@@ -2342,10 +2343,10 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>202212</v>
       </c>
@@ -2353,7 +2354,7 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -2362,14 +2363,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53BFC40-EBB5-4CD8-A1BF-227F8B7027B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2383,7 +2384,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>202200</v>
       </c>
@@ -2394,10 +2395,10 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>202201</v>
       </c>
@@ -2408,10 +2409,10 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>202202</v>
       </c>
@@ -2422,10 +2423,10 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>202203</v>
       </c>
@@ -2436,10 +2437,10 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>202204</v>
       </c>
@@ -2450,10 +2451,10 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>202205</v>
       </c>
@@ -2464,10 +2465,10 @@
         <v>11</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>202206</v>
       </c>
@@ -2478,10 +2479,10 @@
         <v>11</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>202207</v>
       </c>
@@ -2492,10 +2493,10 @@
         <v>11</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>202208</v>
       </c>
@@ -2506,10 +2507,10 @@
         <v>11</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>202209</v>
       </c>
@@ -2520,10 +2521,10 @@
         <v>11</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>202210</v>
       </c>
@@ -2534,10 +2535,10 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>202211</v>
       </c>
@@ -2548,10 +2549,10 @@
         <v>11</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>202212</v>
       </c>
@@ -2562,10 +2563,10 @@
         <v>11</v>
       </c>
       <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>202200</v>
       </c>
@@ -2576,10 +2577,10 @@
         <v>12</v>
       </c>
       <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>202201</v>
       </c>
@@ -2590,10 +2591,10 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.500000000000114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>202202</v>
       </c>
@@ -2604,10 +2605,10 @@
         <v>12</v>
       </c>
       <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>202203</v>
       </c>
@@ -2618,10 +2619,10 @@
         <v>12</v>
       </c>
       <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>202204</v>
       </c>
@@ -2632,10 +2633,10 @@
         <v>12</v>
       </c>
       <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>202205</v>
       </c>
@@ -2646,10 +2647,10 @@
         <v>12</v>
       </c>
       <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>202206</v>
       </c>
@@ -2660,10 +2661,10 @@
         <v>12</v>
       </c>
       <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>202207</v>
       </c>
@@ -2674,10 +2675,10 @@
         <v>12</v>
       </c>
       <c r="D22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>202208</v>
       </c>
@@ -2688,10 +2689,10 @@
         <v>12</v>
       </c>
       <c r="D23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>202209</v>
       </c>
@@ -2702,10 +2703,10 @@
         <v>12</v>
       </c>
       <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>202210</v>
       </c>
@@ -2716,10 +2717,10 @@
         <v>12</v>
       </c>
       <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>202211</v>
       </c>
@@ -2730,10 +2731,10 @@
         <v>12</v>
       </c>
       <c r="D26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>202212</v>
       </c>
@@ -2744,7 +2745,7 @@
         <v>12</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -2753,14 +2754,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947DCEC6-4E7B-478C-816E-FD0496046CA6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2768,20 +2769,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -2790,16 +2791,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77907262-65AD-41B2-AAF9-89C3BD1E8FDE}">
-  <dimension ref="A1:D37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2824,10 +2823,10 @@
         <v>202201</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2838,10 +2837,10 @@
         <v>202201</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2852,26 +2851,26 @@
         <v>202201</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>202201</v>
+      </c>
+      <c r="D5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>202202</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -2880,12 +2879,12 @@
         <v>202202</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -2894,40 +2893,40 @@
         <v>202202</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>202202</v>
+      </c>
+      <c r="D8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>202202</v>
+      </c>
+      <c r="D9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>202203</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>202203</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -2936,52 +2935,52 @@
         <v>202203</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11">
-        <v>202204</v>
+        <v>202203</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12">
-        <v>202204</v>
+        <v>202203</v>
       </c>
       <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13">
-        <v>202204</v>
+        <v>202203</v>
       </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2989,13 +2988,13 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>202205</v>
+        <v>202204</v>
       </c>
       <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -3003,13 +3002,13 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>202205</v>
+        <v>202204</v>
       </c>
       <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -3017,139 +3016,139 @@
         <v>14</v>
       </c>
       <c r="C16">
+        <v>202204</v>
+      </c>
+      <c r="D16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>202204</v>
+      </c>
+      <c r="D17">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
         <v>202205</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D18">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>202205</v>
+      </c>
+      <c r="D19">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>202205</v>
+      </c>
+      <c r="D20">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>202205</v>
+      </c>
+      <c r="D21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22">
         <v>202206</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D22">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23">
         <v>202206</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D23">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24">
         <v>202206</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20">
-        <v>202207</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21">
-        <v>202207</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <v>202207</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23">
-        <v>202208</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24">
-        <v>202208</v>
-      </c>
       <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>14</v>
       </c>
       <c r="C25">
-        <v>202208</v>
+        <v>202206</v>
       </c>
       <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -3157,13 +3156,13 @@
         <v>14</v>
       </c>
       <c r="C26">
-        <v>202209</v>
+        <v>202207</v>
       </c>
       <c r="D26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -3171,13 +3170,13 @@
         <v>14</v>
       </c>
       <c r="C27">
-        <v>202209</v>
+        <v>202207</v>
       </c>
       <c r="D27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -3185,136 +3184,304 @@
         <v>14</v>
       </c>
       <c r="C28">
+        <v>202207</v>
+      </c>
+      <c r="D28">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>202207</v>
+      </c>
+      <c r="D29">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30">
+        <v>202208</v>
+      </c>
+      <c r="D30">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>202208</v>
+      </c>
+      <c r="D31">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>202208</v>
+      </c>
+      <c r="D32">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>202208</v>
+      </c>
+      <c r="D33">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34">
         <v>202209</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="D34">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <v>202209</v>
+      </c>
+      <c r="D35">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <v>202209</v>
+      </c>
+      <c r="D36">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>202209</v>
+      </c>
+      <c r="D37">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>18</v>
       </c>
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29">
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38">
         <v>202210</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="D38">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
         <v>19</v>
       </c>
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30">
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39">
         <v>202210</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="D39">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
         <v>20</v>
       </c>
-      <c r="B31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31">
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40">
         <v>202210</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="D40">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <v>202210</v>
+      </c>
+      <c r="D41">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
         <v>18</v>
       </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32">
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42">
         <v>202211</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D42">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>19</v>
       </c>
-      <c r="B33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33">
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43">
         <v>202211</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D43">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
         <v>20</v>
       </c>
-      <c r="B34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34">
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44">
         <v>202211</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="D44">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45">
+        <v>202211</v>
+      </c>
+      <c r="D45">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
         <v>18</v>
       </c>
-      <c r="B35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35">
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46">
         <v>202212</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D46">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
         <v>19</v>
       </c>
-      <c r="B36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36">
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47">
         <v>202212</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="D47">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
         <v>20</v>
       </c>
-      <c r="B37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37">
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48">
         <v>202212</v>
       </c>
-      <c r="D37">
-        <v>1</v>
+      <c r="D48">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49">
+        <v>202212</v>
+      </c>
+      <c r="D49">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -3323,14 +3490,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD90FB7-F53A-4DE6-8299-4D57AC1D654F}">
-  <dimension ref="A1:D37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3344,7 +3511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3355,10 +3522,10 @@
         <v>202201</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3369,10 +3536,10 @@
         <v>202201</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -3383,26 +3550,26 @@
         <v>202201</v>
       </c>
       <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>202201</v>
+      </c>
+      <c r="D5">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>202202</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -3411,12 +3578,12 @@
         <v>202202</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -3425,40 +3592,40 @@
         <v>202202</v>
       </c>
       <c r="D7">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>202202</v>
+      </c>
+      <c r="D8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>202202</v>
+      </c>
+      <c r="D9">
+        <v>45.999999999999886</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>202203</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>202203</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -3467,52 +3634,52 @@
         <v>202203</v>
       </c>
       <c r="D10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11">
-        <v>202204</v>
+        <v>202203</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12">
-        <v>202204</v>
+        <v>202203</v>
       </c>
       <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13">
-        <v>202204</v>
+        <v>202203</v>
       </c>
       <c r="D13">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -3520,13 +3687,13 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>202205</v>
+        <v>202204</v>
       </c>
       <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -3534,13 +3701,13 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>202205</v>
+        <v>202204</v>
       </c>
       <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -3548,139 +3715,139 @@
         <v>14</v>
       </c>
       <c r="C16">
+        <v>202204</v>
+      </c>
+      <c r="D16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>202204</v>
+      </c>
+      <c r="D17">
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
         <v>202205</v>
       </c>
-      <c r="D16">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D18">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>202205</v>
+      </c>
+      <c r="D19">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>202205</v>
+      </c>
+      <c r="D20">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>202205</v>
+      </c>
+      <c r="D21">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22">
         <v>202206</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D22">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23">
         <v>202206</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D23">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24">
         <v>202206</v>
       </c>
-      <c r="D19">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20">
-        <v>202207</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21">
-        <v>202207</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <v>202207</v>
-      </c>
-      <c r="D22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23">
-        <v>202208</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24">
-        <v>202208</v>
-      </c>
       <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>14</v>
       </c>
       <c r="C25">
-        <v>202208</v>
+        <v>202206</v>
       </c>
       <c r="D25">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -3688,13 +3855,13 @@
         <v>14</v>
       </c>
       <c r="C26">
-        <v>202209</v>
+        <v>202207</v>
       </c>
       <c r="D26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -3702,13 +3869,13 @@
         <v>14</v>
       </c>
       <c r="C27">
-        <v>202209</v>
+        <v>202207</v>
       </c>
       <c r="D27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -3716,136 +3883,472 @@
         <v>14</v>
       </c>
       <c r="C28">
+        <v>202207</v>
+      </c>
+      <c r="D28">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>202207</v>
+      </c>
+      <c r="D29">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30">
+        <v>202208</v>
+      </c>
+      <c r="D30">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>202208</v>
+      </c>
+      <c r="D31">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>202208</v>
+      </c>
+      <c r="D32">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>202208</v>
+      </c>
+      <c r="D33">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34">
         <v>202209</v>
       </c>
-      <c r="D28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="D34">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <v>202209</v>
+      </c>
+      <c r="D35">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <v>202209</v>
+      </c>
+      <c r="D36">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>202209</v>
+      </c>
+      <c r="D37">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>18</v>
       </c>
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29">
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38">
         <v>202210</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="D38">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
         <v>19</v>
       </c>
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30">
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39">
         <v>202210</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="D39">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
         <v>20</v>
       </c>
-      <c r="B31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31">
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40">
         <v>202210</v>
       </c>
-      <c r="D31">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="D40">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <v>202210</v>
+      </c>
+      <c r="D41">
+        <v>86.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
         <v>18</v>
       </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32">
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42">
         <v>202211</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D42">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>19</v>
       </c>
-      <c r="B33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33">
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43">
         <v>202211</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D43">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
         <v>20</v>
       </c>
-      <c r="B34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34">
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44">
         <v>202211</v>
       </c>
-      <c r="D34">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="D44">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45">
+        <v>202211</v>
+      </c>
+      <c r="D45">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
         <v>18</v>
       </c>
-      <c r="B35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35">
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46">
         <v>202212</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D46">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
         <v>19</v>
       </c>
-      <c r="B36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36">
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47">
         <v>202212</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="D47">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
         <v>20</v>
       </c>
-      <c r="B37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37">
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48">
         <v>202212</v>
       </c>
-      <c r="D37">
-        <v>10</v>
+      <c r="D48">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49">
+        <v>202212</v>
+      </c>
+      <c r="D49">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50">
+        <v>202213</v>
+      </c>
+      <c r="D50">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51">
+        <v>202213</v>
+      </c>
+      <c r="D51">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52">
+        <v>202213</v>
+      </c>
+      <c r="D52">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53">
+        <v>202213</v>
+      </c>
+      <c r="D53">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54">
+        <v>202214</v>
+      </c>
+      <c r="D54">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55">
+        <v>202214</v>
+      </c>
+      <c r="D55">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56">
+        <v>202214</v>
+      </c>
+      <c r="D56">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57">
+        <v>202214</v>
+      </c>
+      <c r="D57">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58">
+        <v>202215</v>
+      </c>
+      <c r="D58">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59">
+        <v>202215</v>
+      </c>
+      <c r="D59">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60">
+        <v>202215</v>
+      </c>
+      <c r="D60">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61">
+        <v>202215</v>
+      </c>
+      <c r="D61">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
F I N A L L Y ! !
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Thesis\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E542250-ECE1-4660-8F2D-368A688ACC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
-    <sheet name="Inventory" r:id="rId5" sheetId="2"/>
-    <sheet name="RawMaterialInventory" r:id="rId6" sheetId="3"/>
-    <sheet name="PMRunning" r:id="rId7" sheetId="4"/>
-    <sheet name="Contracts" r:id="rId8" sheetId="5"/>
-    <sheet name="RawMaterialContract" r:id="rId9" sheetId="6"/>
-    <sheet name="RawMaterialPrices" r:id="rId10" sheetId="7"/>
+    <sheet name="Inventory" sheetId="2" r:id="rId2"/>
+    <sheet name="RawMaterialInventory" sheetId="3" r:id="rId3"/>
+    <sheet name="PMRunning" sheetId="4" r:id="rId4"/>
+    <sheet name="Contracts" sheetId="5" r:id="rId5"/>
+    <sheet name="RawMaterialContract" sheetId="6" r:id="rId6"/>
+    <sheet name="RawMaterialPrices" sheetId="7" r:id="rId7"/>
+    <sheet name="FD_Costs" sheetId="8" r:id="rId8"/>
+    <sheet name="Slack32" sheetId="9" r:id="rId9"/>
+    <sheet name="Slack31" sheetId="10" r:id="rId10"/>
+    <sheet name="Slack21" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="25">
   <si>
     <t>Product</t>
   </si>
@@ -456,14 +460,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC741EA-9077-4DFF-94A3-559830F16352}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -500,10 +504,10 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>330.7670569961674</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>331.99225389493779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -520,10 +524,10 @@
         <v>9</v>
       </c>
       <c r="F3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>36.671501241192516</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -540,10 +544,10 @@
         <v>9</v>
       </c>
       <c r="F4">
-        <v>56.00141939211461</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>204.27999651623821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -560,10 +564,10 @@
         <v>9</v>
       </c>
       <c r="F5">
-        <v>1636.2038144547173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>45.555303666099313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -580,10 +584,10 @@
         <v>9</v>
       </c>
       <c r="F6">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>173.3267269583655</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -600,10 +604,10 @@
         <v>9</v>
       </c>
       <c r="F7">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>4.36399127915662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -620,10 +624,10 @@
         <v>9</v>
       </c>
       <c r="F8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>249.93622941726181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -640,10 +644,10 @@
         <v>9</v>
       </c>
       <c r="F9">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>282.33220504754468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -660,10 +664,10 @@
         <v>9</v>
       </c>
       <c r="F10">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -680,10 +684,10 @@
         <v>9</v>
       </c>
       <c r="F11">
-        <v>161.58913432915932</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>130.71381309533626</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -700,10 +704,10 @@
         <v>9</v>
       </c>
       <c r="F12">
-        <v>394.12060815196384</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -720,7 +724,481 @@
         <v>9</v>
       </c>
       <c r="F13">
-        <v>0.0</v>
+        <v>1.966193085373753</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2114CC-7A79-4E79-BA3E-8EB8A127A395}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>202101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>202102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>202103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>202104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>202105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>202106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>202107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>202108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>202109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>202110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>202111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>202112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>202113</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>202114</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>202115</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDD91CE-DB54-4B48-81E2-F0144D749612}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>202101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>202102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>202103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>202104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>202105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>202106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>202107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>202108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>202109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>202110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>202111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>202112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>202113</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>202114</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>202115</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -729,14 +1207,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5715696D-DC9A-4BFD-8538-FAFE15C5253A}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -756,7 +1234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -773,10 +1251,10 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -793,10 +1271,10 @@
         <v>9</v>
       </c>
       <c r="F3">
-        <v>57.32794381991783</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>212.92474281182467</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -813,10 +1291,10 @@
         <v>9</v>
       </c>
       <c r="F4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -833,10 +1311,10 @@
         <v>9</v>
       </c>
       <c r="F5">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -853,10 +1331,10 @@
         <v>9</v>
       </c>
       <c r="F6">
-        <v>1276.5444609664842</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -873,10 +1351,10 @@
         <v>9</v>
       </c>
       <c r="F7">
-        <v>928.1530869290414</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -893,10 +1371,10 @@
         <v>9</v>
       </c>
       <c r="F8">
-        <v>921.7203634973434</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -913,10 +1391,10 @@
         <v>9</v>
       </c>
       <c r="F9">
-        <v>604.2767672228056</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -933,10 +1411,10 @@
         <v>9</v>
       </c>
       <c r="F10">
-        <v>311.1496969441456</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>282.09560649169401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -953,10 +1431,10 @@
         <v>9</v>
       </c>
       <c r="F11">
-        <v>231.88289587228326</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>33.67208170458332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -973,10 +1451,10 @@
         <v>9</v>
       </c>
       <c r="F12">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>153.73357771541231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -993,10 +1471,10 @@
         <v>9</v>
       </c>
       <c r="F13">
-        <v>393.4699122621148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1013,7 +1491,7 @@
         <v>9</v>
       </c>
       <c r="F14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1022,14 +1500,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E5B8F58-BAE0-4932-B85D-36799FAF77EA}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1046,7 +1524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>202100</v>
       </c>
@@ -1060,10 +1538,10 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>202101</v>
       </c>
@@ -1077,10 +1555,10 @@
         <v>9</v>
       </c>
       <c r="E3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>202102</v>
       </c>
@@ -1094,10 +1572,10 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>83.804247637520419</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>202103</v>
       </c>
@@ -1111,10 +1589,10 @@
         <v>9</v>
       </c>
       <c r="E5">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>202104</v>
       </c>
@@ -1128,10 +1606,10 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>121.44668883646523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>202105</v>
       </c>
@@ -1145,10 +1623,10 @@
         <v>9</v>
       </c>
       <c r="E7">
-        <v>555.7097424811232</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>202106</v>
       </c>
@@ -1162,10 +1640,10 @@
         <v>9</v>
       </c>
       <c r="E8">
-        <v>555.7097424811232</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>47.516046842743421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>202107</v>
       </c>
@@ -1179,10 +1657,10 @@
         <v>9</v>
       </c>
       <c r="E9">
-        <v>555.7097424811232</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>151.61839195220841</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>202108</v>
       </c>
@@ -1196,10 +1674,10 @@
         <v>9</v>
       </c>
       <c r="E10">
-        <v>555.7097424811232</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>202109</v>
       </c>
@@ -1213,10 +1691,10 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>555.7097424811232</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>130.71381309533626</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>202110</v>
       </c>
@@ -1230,10 +1708,10 @@
         <v>9</v>
       </c>
       <c r="E12">
-        <v>394.12060815196384</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>202111</v>
       </c>
@@ -1247,10 +1725,10 @@
         <v>9</v>
       </c>
       <c r="E13">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>202112</v>
       </c>
@@ -1264,7 +1742,7 @@
         <v>9</v>
       </c>
       <c r="E14">
-        <v>0.0</v>
+        <v>89.640332717189068</v>
       </c>
     </row>
   </sheetData>
@@ -1273,14 +1751,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FA6021-2F31-4193-92AF-B0A216A985A1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1291,7 +1769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1299,7 +1777,7 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1308,14 +1786,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:E49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD9D70D-7CE1-47A4-BACF-3AD106FCF0F4}">
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1332,7 +1810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1346,10 +1824,10 @@
         <v>11</v>
       </c>
       <c r="E2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1363,10 +1841,10 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1380,10 +1858,10 @@
         <v>11</v>
       </c>
       <c r="E4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1397,10 +1875,10 @@
         <v>11</v>
       </c>
       <c r="E5">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1414,10 +1892,10 @@
         <v>11</v>
       </c>
       <c r="E6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1431,10 +1909,10 @@
         <v>11</v>
       </c>
       <c r="E7">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1448,10 +1926,10 @@
         <v>11</v>
       </c>
       <c r="E8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1465,10 +1943,10 @@
         <v>11</v>
       </c>
       <c r="E9">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1482,10 +1960,10 @@
         <v>11</v>
       </c>
       <c r="E10">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1499,10 +1977,10 @@
         <v>11</v>
       </c>
       <c r="E11">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1516,10 +1994,10 @@
         <v>11</v>
       </c>
       <c r="E12">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1533,10 +2011,10 @@
         <v>11</v>
       </c>
       <c r="E13">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1550,10 +2028,10 @@
         <v>11</v>
       </c>
       <c r="E14">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1567,10 +2045,10 @@
         <v>11</v>
       </c>
       <c r="E15">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1584,10 +2062,10 @@
         <v>11</v>
       </c>
       <c r="E16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1601,10 +2079,10 @@
         <v>11</v>
       </c>
       <c r="E17">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1618,10 +2096,10 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1635,10 +2113,10 @@
         <v>11</v>
       </c>
       <c r="E19">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1652,10 +2130,10 @@
         <v>11</v>
       </c>
       <c r="E20">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1669,10 +2147,10 @@
         <v>11</v>
       </c>
       <c r="E21">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1686,10 +2164,10 @@
         <v>11</v>
       </c>
       <c r="E22">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1703,10 +2181,10 @@
         <v>11</v>
       </c>
       <c r="E23">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1720,10 +2198,10 @@
         <v>11</v>
       </c>
       <c r="E24">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1737,10 +2215,10 @@
         <v>11</v>
       </c>
       <c r="E25">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1754,10 +2232,10 @@
         <v>11</v>
       </c>
       <c r="E26">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1771,10 +2249,10 @@
         <v>11</v>
       </c>
       <c r="E27">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -1788,10 +2266,10 @@
         <v>11</v>
       </c>
       <c r="E28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1805,10 +2283,10 @@
         <v>11</v>
       </c>
       <c r="E29">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1822,10 +2300,10 @@
         <v>11</v>
       </c>
       <c r="E30">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -1839,10 +2317,10 @@
         <v>11</v>
       </c>
       <c r="E31">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1856,10 +2334,10 @@
         <v>11</v>
       </c>
       <c r="E32">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1873,10 +2351,10 @@
         <v>11</v>
       </c>
       <c r="E33">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1890,10 +2368,10 @@
         <v>11</v>
       </c>
       <c r="E34">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1907,10 +2385,10 @@
         <v>11</v>
       </c>
       <c r="E35">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -1924,10 +2402,10 @@
         <v>11</v>
       </c>
       <c r="E36">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -1941,10 +2419,10 @@
         <v>11</v>
       </c>
       <c r="E37">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1958,10 +2436,10 @@
         <v>11</v>
       </c>
       <c r="E38">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -1975,10 +2453,10 @@
         <v>11</v>
       </c>
       <c r="E39">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1992,10 +2470,10 @@
         <v>11</v>
       </c>
       <c r="E40">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -2009,10 +2487,10 @@
         <v>11</v>
       </c>
       <c r="E41">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -2026,10 +2504,10 @@
         <v>11</v>
       </c>
       <c r="E42">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -2043,10 +2521,10 @@
         <v>11</v>
       </c>
       <c r="E43">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -2060,10 +2538,10 @@
         <v>11</v>
       </c>
       <c r="E44">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -2077,10 +2555,10 @@
         <v>11</v>
       </c>
       <c r="E45">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -2094,10 +2572,10 @@
         <v>11</v>
       </c>
       <c r="E46">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2111,10 +2589,10 @@
         <v>11</v>
       </c>
       <c r="E47">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -2128,10 +2606,10 @@
         <v>11</v>
       </c>
       <c r="E48">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>20</v>
       </c>
@@ -2145,7 +2623,211 @@
         <v>11</v>
       </c>
       <c r="E49">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50">
+        <v>202113</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>202113</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52">
+        <v>202113</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53">
+        <v>202113</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54">
+        <v>202114</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55">
+        <v>202114</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56">
+        <v>202114</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57">
+        <v>202114</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58">
+        <v>202115</v>
+      </c>
+      <c r="D58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59">
+        <v>202115</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60">
+        <v>202115</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61">
+        <v>202115</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2154,14 +2836,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAE2468-C7B5-49D1-878D-18AB2291C50E}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2181,7 +2863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2198,10 +2880,10 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2218,10 +2900,10 @@
         <v>9</v>
       </c>
       <c r="F3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2238,10 +2920,10 @@
         <v>9</v>
       </c>
       <c r="F4">
-        <v>330.7670569961674</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2258,10 +2940,10 @@
         <v>9</v>
       </c>
       <c r="F5">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>331.99225389493779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2278,10 +2960,10 @@
         <v>9</v>
       </c>
       <c r="F6">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2298,10 +2980,10 @@
         <v>9</v>
       </c>
       <c r="F7">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2318,10 +3000,10 @@
         <v>9</v>
       </c>
       <c r="F8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2338,10 +3020,10 @@
         <v>9</v>
       </c>
       <c r="F9">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>120.47574887871292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2358,10 +3040,10 @@
         <v>9</v>
       </c>
       <c r="F10">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2378,10 +3060,10 @@
         <v>9</v>
       </c>
       <c r="F11">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2398,10 +3080,10 @@
         <v>9</v>
       </c>
       <c r="F12">
-        <v>56.001419392114606</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>6.4203237020632728E-12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2418,10 +3100,10 @@
         <v>9</v>
       </c>
       <c r="F13">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>120.47574887871137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2438,10 +3120,10 @@
         <v>9</v>
       </c>
       <c r="F14">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2458,10 +3140,10 @@
         <v>9</v>
       </c>
       <c r="F15">
-        <v>1636.2038144547173</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2478,10 +3160,10 @@
         <v>9</v>
       </c>
       <c r="F16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2498,10 +3180,10 @@
         <v>9</v>
       </c>
       <c r="F17">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>167.00199250256455</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2518,10 +3200,10 @@
         <v>9</v>
       </c>
       <c r="F18">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2538,10 +3220,10 @@
         <v>9</v>
       </c>
       <c r="F19">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2558,10 +3240,10 @@
         <v>9</v>
       </c>
       <c r="F20">
-        <v>555.7097424811232</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2578,10 +3260,10 @@
         <v>9</v>
       </c>
       <c r="F21">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>51.88003812190027</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2598,10 +3280,10 @@
         <v>9</v>
       </c>
       <c r="F22">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2618,10 +3300,10 @@
         <v>9</v>
       </c>
       <c r="F23">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2638,10 +3320,10 @@
         <v>9</v>
       </c>
       <c r="F24">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2658,10 +3340,10 @@
         <v>9</v>
       </c>
       <c r="F25">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>51.880038121900043</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -2678,10 +3360,10 @@
         <v>9</v>
       </c>
       <c r="F26">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -2698,10 +3380,10 @@
         <v>9</v>
       </c>
       <c r="F27">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -2718,10 +3400,10 @@
         <v>9</v>
       </c>
       <c r="F28">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -2738,10 +3420,10 @@
         <v>9</v>
       </c>
       <c r="F29">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>354.03857452672679</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -2758,10 +3440,10 @@
         <v>9</v>
       </c>
       <c r="F30">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2778,10 +3460,10 @@
         <v>9</v>
       </c>
       <c r="F31">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -2798,10 +3480,10 @@
         <v>9</v>
       </c>
       <c r="F32">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -2818,10 +3500,10 @@
         <v>9</v>
       </c>
       <c r="F33">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>130.71381309533626</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -2838,10 +3520,10 @@
         <v>9</v>
       </c>
       <c r="F34">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -2858,10 +3540,10 @@
         <v>9</v>
       </c>
       <c r="F35">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -2878,10 +3560,10 @@
         <v>9</v>
       </c>
       <c r="F36">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -2898,10 +3580,10 @@
         <v>9</v>
       </c>
       <c r="F37">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>130.71381309533626</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -2918,10 +3600,10 @@
         <v>9</v>
       </c>
       <c r="F38">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -2938,10 +3620,10 @@
         <v>9</v>
       </c>
       <c r="F39">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -2958,10 +3640,10 @@
         <v>9</v>
       </c>
       <c r="F40">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -2978,10 +3660,10 @@
         <v>9</v>
       </c>
       <c r="F41">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -2998,10 +3680,10 @@
         <v>9</v>
       </c>
       <c r="F42">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -3018,10 +3700,10 @@
         <v>9</v>
       </c>
       <c r="F43">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -3038,10 +3720,10 @@
         <v>9</v>
       </c>
       <c r="F44">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -3058,10 +3740,10 @@
         <v>9</v>
       </c>
       <c r="F45">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -3078,10 +3760,10 @@
         <v>9</v>
       </c>
       <c r="F46">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -3098,10 +3780,10 @@
         <v>9</v>
       </c>
       <c r="F47">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>91.606525802562828</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -3118,10 +3800,10 @@
         <v>9</v>
       </c>
       <c r="F48">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>20</v>
       </c>
@@ -3138,10 +3820,10 @@
         <v>9</v>
       </c>
       <c r="F49">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -3158,10 +3840,10 @@
         <v>9</v>
       </c>
       <c r="F50">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -3178,10 +3860,10 @@
         <v>9</v>
       </c>
       <c r="F51">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -3198,10 +3880,10 @@
         <v>9</v>
       </c>
       <c r="F52">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>20</v>
       </c>
@@ -3218,10 +3900,10 @@
         <v>9</v>
       </c>
       <c r="F53">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -3238,10 +3920,10 @@
         <v>9</v>
       </c>
       <c r="F54">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -3258,10 +3940,10 @@
         <v>9</v>
       </c>
       <c r="F55">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -3278,10 +3960,10 @@
         <v>9</v>
       </c>
       <c r="F56">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>20</v>
       </c>
@@ -3298,10 +3980,10 @@
         <v>9</v>
       </c>
       <c r="F57">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -3318,10 +4000,10 @@
         <v>9</v>
       </c>
       <c r="F58">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -3338,10 +4020,10 @@
         <v>9</v>
       </c>
       <c r="F59">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -3358,10 +4040,10 @@
         <v>9</v>
       </c>
       <c r="F60">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>20</v>
       </c>
@@ -3378,7 +4060,7 @@
         <v>9</v>
       </c>
       <c r="F61">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3387,14 +4069,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D3398F-F45C-49FF-ACD3-8A65AC55B84C}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3408,7 +4090,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>202101</v>
       </c>
@@ -3419,10 +4101,10 @@
         <v>9</v>
       </c>
       <c r="D2">
-        <v>71.63104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>71.631039999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>202102</v>
       </c>
@@ -3433,10 +4115,10 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>71.23341</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>72.369500000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>202103</v>
       </c>
@@ -3447,10 +4129,10 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>71.51743</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>70.949380000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>202104</v>
       </c>
@@ -3461,10 +4143,10 @@
         <v>9</v>
       </c>
       <c r="D5">
-        <v>54.19192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>72.710329999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>202105</v>
       </c>
@@ -3475,10 +4157,10 @@
         <v>9</v>
       </c>
       <c r="D6">
-        <v>55.66885</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>70.381330000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>202106</v>
       </c>
@@ -3489,10 +4171,10 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <v>57.03217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>72.483109999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>202107</v>
       </c>
@@ -3503,10 +4185,10 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>66.91623</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>66.291380000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>202108</v>
       </c>
@@ -3517,10 +4199,10 @@
         <v>9</v>
       </c>
       <c r="D9">
-        <v>67.7683</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>67.029839999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>202109</v>
       </c>
@@ -3531,10 +4213,10 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>68.16594</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>66.916229999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>202110</v>
       </c>
@@ -3545,10 +4227,10 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>55.66885</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>67.257059999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>202111</v>
       </c>
@@ -3559,10 +4241,10 @@
         <v>9</v>
       </c>
       <c r="D12">
-        <v>57.03217</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>66.404989999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>202112</v>
       </c>
@@ -3573,7 +4255,529 @@
         <v>9</v>
       </c>
       <c r="D13">
-        <v>57.54341</v>
+        <v>66.916229999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693FEB75-BCED-4B8F-B053-7F1A14B43B8C}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>202101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>16969.572829740264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>202102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>6158.0412519563406</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>202103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>6158.0412519562615</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>202104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>7285.8723228926519</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>202105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>2263.3941559539435</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>202106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>2263.3941559539335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>202107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>15152.859224883816</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>202108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>5594.5542409585096</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>202109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>5594.5542409585105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>202110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>202111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>202112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>202113</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>202114</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>202115</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29922CDA-5F5F-4171-813F-79224B952DC5}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>202101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>202102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>202103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>202104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>202105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>202106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>202107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>202108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>202109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>202110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>202111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>202112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>202113</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>202114</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>202115</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>